<commit_message>
trimming extra lines from blank, since formulas are being input fine.
</commit_message>
<xml_diff>
--- a/data/wip_blank.xlsx
+++ b/data/wip_blank.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25819"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://windlecc-my.sharepoint.com/personal/sung_windlecc_com/Documents/QuickBooks Related/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0AD2CEAB-D046-4F70-97B4-6B3C1D1D471A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B622D537-DEBD-40E2-8E0E-7A79A54E957F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6735" yWindow="0" windowWidth="20820" windowHeight="14460" xr2:uid="{DA826FD3-3801-4C58-8C10-4349DA3C3603}"/>
   </bookViews>
@@ -1058,8 +1058,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99DDC2FF-48ED-455E-AE3E-AFE8DEE19056}">
   <dimension ref="A1:V63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="V5" sqref="V5"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7:Q53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1320,42 +1320,18 @@
       <c r="C7" s="12"/>
       <c r="D7" s="32"/>
       <c r="E7" s="32"/>
-      <c r="F7" s="108">
-        <f>D7+E7</f>
-        <v>0</v>
-      </c>
+      <c r="F7" s="108"/>
       <c r="G7" s="126"/>
-      <c r="H7" s="9">
-        <f t="shared" ref="H7:H53" si="0">+F7-G7</f>
-        <v>0</v>
-      </c>
-      <c r="I7" s="94" t="e">
-        <f t="shared" ref="I7:I52" si="1">H7/G7</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="H7" s="9"/>
+      <c r="I7" s="94"/>
       <c r="J7" s="32"/>
-      <c r="K7" s="100" t="e">
-        <f t="shared" ref="K7:K52" si="2">+J7/G7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L7" s="9" t="e">
-        <f t="shared" ref="L7:L52" si="3">F7*K7</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="K7" s="100"/>
+      <c r="L7" s="9"/>
       <c r="M7" s="32"/>
       <c r="N7" s="16"/>
-      <c r="O7" s="9" t="e">
-        <f t="shared" ref="O7" si="4">IF(L7&gt;M7,L7-M7,IF((L7-M7)&lt;-1,"-",0))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P7" s="9" t="e">
-        <f t="shared" ref="P7" si="5">IF(L7&gt;M7,"-",L7-M7)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q7" s="9" t="e">
-        <f t="shared" ref="Q7" si="6">+F7-L7</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9"/>
       <c r="R7" s="56"/>
       <c r="S7" s="42"/>
       <c r="T7" s="42"/>
@@ -1368,42 +1344,18 @@
       <c r="C8" s="7"/>
       <c r="D8" s="33"/>
       <c r="E8" s="33"/>
-      <c r="F8" s="108">
-        <f t="shared" ref="F8:F52" si="7">D8+E8</f>
-        <v>0</v>
-      </c>
+      <c r="F8" s="108"/>
       <c r="G8" s="127"/>
-      <c r="H8" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I8" s="94" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="H8" s="9"/>
+      <c r="I8" s="94"/>
       <c r="J8" s="33"/>
-      <c r="K8" s="100" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L8" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="K8" s="100"/>
+      <c r="L8" s="9"/>
       <c r="M8" s="33"/>
       <c r="N8" s="9"/>
-      <c r="O8" s="9" t="e">
-        <f t="shared" ref="O8:O29" si="8">IF(L8&gt;M8,L8-M8,IF((L8-M8)&lt;-1,"-",0))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P8" s="9" t="e">
-        <f t="shared" ref="P8:P29" si="9">IF(L8&gt;M8,"-",L8-M8)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q8" s="9" t="e">
-        <f t="shared" ref="Q8:Q29" si="10">+F8-L8</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
       <c r="R8" s="57"/>
       <c r="S8" s="43"/>
       <c r="T8" s="43"/>
@@ -1416,42 +1368,18 @@
       <c r="C9" s="17"/>
       <c r="D9" s="34"/>
       <c r="E9" s="34"/>
-      <c r="F9" s="108">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
+      <c r="F9" s="108"/>
       <c r="G9" s="128"/>
-      <c r="H9" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I9" s="94" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="H9" s="9"/>
+      <c r="I9" s="94"/>
       <c r="J9" s="34"/>
-      <c r="K9" s="100" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L9" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="K9" s="100"/>
+      <c r="L9" s="9"/>
       <c r="M9" s="34"/>
       <c r="N9" s="18"/>
-      <c r="O9" s="9" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P9" s="9" t="e">
-        <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q9" s="9" t="e">
-        <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9"/>
       <c r="R9" s="58"/>
       <c r="S9" s="44"/>
       <c r="T9" s="44"/>
@@ -1464,42 +1392,18 @@
       <c r="C10" s="7"/>
       <c r="D10" s="33"/>
       <c r="E10" s="33"/>
-      <c r="F10" s="108">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
+      <c r="F10" s="108"/>
       <c r="G10" s="127"/>
-      <c r="H10" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I10" s="94" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="H10" s="9"/>
+      <c r="I10" s="94"/>
       <c r="J10" s="33"/>
-      <c r="K10" s="100" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L10" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="K10" s="100"/>
+      <c r="L10" s="9"/>
       <c r="M10" s="33"/>
       <c r="N10" s="9"/>
-      <c r="O10" s="9" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P10" s="9" t="e">
-        <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q10" s="9" t="e">
-        <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="9"/>
       <c r="R10" s="57"/>
       <c r="S10" s="43"/>
       <c r="T10" s="43"/>
@@ -1512,42 +1416,18 @@
       <c r="C11" s="7"/>
       <c r="D11" s="33"/>
       <c r="E11" s="33"/>
-      <c r="F11" s="108">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
+      <c r="F11" s="108"/>
       <c r="G11" s="127"/>
-      <c r="H11" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I11" s="94" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="H11" s="9"/>
+      <c r="I11" s="94"/>
       <c r="J11" s="33"/>
-      <c r="K11" s="100" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L11" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="K11" s="100"/>
+      <c r="L11" s="9"/>
       <c r="M11" s="33"/>
       <c r="N11" s="9"/>
-      <c r="O11" s="9" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P11" s="9" t="e">
-        <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q11" s="9" t="e">
-        <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="9"/>
       <c r="R11" s="57"/>
       <c r="S11" s="43"/>
       <c r="T11" s="43"/>
@@ -1560,42 +1440,18 @@
       <c r="C12" s="7"/>
       <c r="D12" s="33"/>
       <c r="E12" s="33"/>
-      <c r="F12" s="108">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
+      <c r="F12" s="108"/>
       <c r="G12" s="127"/>
-      <c r="H12" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I12" s="94" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="H12" s="9"/>
+      <c r="I12" s="94"/>
       <c r="J12" s="33"/>
-      <c r="K12" s="100" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L12" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="K12" s="100"/>
+      <c r="L12" s="9"/>
       <c r="M12" s="33"/>
       <c r="N12" s="9"/>
-      <c r="O12" s="9" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P12" s="9" t="e">
-        <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q12" s="9" t="e">
-        <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="O12" s="9"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="9"/>
       <c r="R12" s="57"/>
       <c r="S12" s="43"/>
       <c r="T12" s="43"/>
@@ -1608,42 +1464,18 @@
       <c r="C13" s="7"/>
       <c r="D13" s="33"/>
       <c r="E13" s="33"/>
-      <c r="F13" s="108">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
+      <c r="F13" s="108"/>
       <c r="G13" s="127"/>
-      <c r="H13" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I13" s="94" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="H13" s="9"/>
+      <c r="I13" s="94"/>
       <c r="J13" s="33"/>
-      <c r="K13" s="100" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L13" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="K13" s="100"/>
+      <c r="L13" s="9"/>
       <c r="M13" s="33"/>
       <c r="N13" s="9"/>
-      <c r="O13" s="9" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P13" s="9" t="e">
-        <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q13" s="9" t="e">
-        <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="9"/>
       <c r="R13" s="57"/>
       <c r="S13" s="43"/>
       <c r="T13" s="43"/>
@@ -1656,42 +1488,18 @@
       <c r="C14" s="7"/>
       <c r="D14" s="33"/>
       <c r="E14" s="33"/>
-      <c r="F14" s="108">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
+      <c r="F14" s="108"/>
       <c r="G14" s="127"/>
-      <c r="H14" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I14" s="94" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="H14" s="9"/>
+      <c r="I14" s="94"/>
       <c r="J14" s="33"/>
-      <c r="K14" s="100" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L14" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="K14" s="100"/>
+      <c r="L14" s="9"/>
       <c r="M14" s="33"/>
       <c r="N14" s="9"/>
-      <c r="O14" s="9" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P14" s="9" t="e">
-        <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q14" s="9" t="e">
-        <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="O14" s="9"/>
+      <c r="P14" s="9"/>
+      <c r="Q14" s="9"/>
       <c r="R14" s="57"/>
       <c r="S14" s="43"/>
       <c r="T14" s="43"/>
@@ -1704,42 +1512,18 @@
       <c r="C15" s="7"/>
       <c r="D15" s="33"/>
       <c r="E15" s="33"/>
-      <c r="F15" s="108">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
+      <c r="F15" s="108"/>
       <c r="G15" s="127"/>
-      <c r="H15" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I15" s="94" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="H15" s="9"/>
+      <c r="I15" s="94"/>
       <c r="J15" s="33"/>
-      <c r="K15" s="100" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L15" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="K15" s="100"/>
+      <c r="L15" s="9"/>
       <c r="M15" s="33"/>
       <c r="N15" s="9"/>
-      <c r="O15" s="9" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P15" s="9" t="e">
-        <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q15" s="9" t="e">
-        <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="O15" s="9"/>
+      <c r="P15" s="9"/>
+      <c r="Q15" s="9"/>
       <c r="R15" s="57"/>
       <c r="S15" s="43"/>
       <c r="T15" s="43"/>
@@ -1752,42 +1536,18 @@
       <c r="C16" s="7"/>
       <c r="D16" s="33"/>
       <c r="E16" s="33"/>
-      <c r="F16" s="108">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
+      <c r="F16" s="108"/>
       <c r="G16" s="127"/>
-      <c r="H16" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I16" s="94" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="H16" s="9"/>
+      <c r="I16" s="94"/>
       <c r="J16" s="33"/>
-      <c r="K16" s="100" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L16" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="K16" s="100"/>
+      <c r="L16" s="9"/>
       <c r="M16" s="33"/>
       <c r="N16" s="9"/>
-      <c r="O16" s="9" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P16" s="9" t="e">
-        <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q16" s="9" t="e">
-        <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="O16" s="9"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="9"/>
       <c r="R16" s="57"/>
       <c r="S16" s="43"/>
       <c r="T16" s="43"/>
@@ -1800,42 +1560,18 @@
       <c r="C17" s="7"/>
       <c r="D17" s="33"/>
       <c r="E17" s="33"/>
-      <c r="F17" s="108">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
+      <c r="F17" s="108"/>
       <c r="G17" s="127"/>
-      <c r="H17" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I17" s="94" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="H17" s="9"/>
+      <c r="I17" s="94"/>
       <c r="J17" s="33"/>
-      <c r="K17" s="100" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L17" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="K17" s="100"/>
+      <c r="L17" s="9"/>
       <c r="M17" s="33"/>
       <c r="N17" s="9"/>
-      <c r="O17" s="9" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P17" s="9" t="e">
-        <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q17" s="9" t="e">
-        <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="O17" s="9"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="9"/>
       <c r="R17" s="57"/>
       <c r="S17" s="43"/>
       <c r="T17" s="43"/>
@@ -1848,42 +1584,18 @@
       <c r="C18" s="7"/>
       <c r="D18" s="33"/>
       <c r="E18" s="33"/>
-      <c r="F18" s="108">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
+      <c r="F18" s="108"/>
       <c r="G18" s="127"/>
-      <c r="H18" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I18" s="94" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="H18" s="9"/>
+      <c r="I18" s="94"/>
       <c r="J18" s="33"/>
-      <c r="K18" s="100" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L18" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="K18" s="100"/>
+      <c r="L18" s="9"/>
       <c r="M18" s="33"/>
       <c r="N18" s="9"/>
-      <c r="O18" s="9" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P18" s="9" t="e">
-        <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q18" s="9" t="e">
-        <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="O18" s="9"/>
+      <c r="P18" s="9"/>
+      <c r="Q18" s="9"/>
       <c r="R18" s="57"/>
       <c r="S18" s="43"/>
       <c r="T18" s="43"/>
@@ -1896,42 +1608,18 @@
       <c r="C19" s="7"/>
       <c r="D19" s="33"/>
       <c r="E19" s="33"/>
-      <c r="F19" s="108">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
+      <c r="F19" s="108"/>
       <c r="G19" s="127"/>
-      <c r="H19" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I19" s="94" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="H19" s="9"/>
+      <c r="I19" s="94"/>
       <c r="J19" s="33"/>
-      <c r="K19" s="100" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L19" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="K19" s="100"/>
+      <c r="L19" s="9"/>
       <c r="M19" s="33"/>
       <c r="N19" s="9"/>
-      <c r="O19" s="9" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P19" s="9" t="e">
-        <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q19" s="9" t="e">
-        <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="O19" s="9"/>
+      <c r="P19" s="9"/>
+      <c r="Q19" s="9"/>
       <c r="R19" s="57"/>
       <c r="S19" s="43"/>
       <c r="T19" s="43"/>
@@ -1944,42 +1632,18 @@
       <c r="C20" s="19"/>
       <c r="D20" s="33"/>
       <c r="E20" s="33"/>
-      <c r="F20" s="108">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
+      <c r="F20" s="108"/>
       <c r="G20" s="127"/>
-      <c r="H20" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I20" s="94" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="H20" s="9"/>
+      <c r="I20" s="94"/>
       <c r="J20" s="33"/>
-      <c r="K20" s="100" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L20" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="K20" s="100"/>
+      <c r="L20" s="9"/>
       <c r="M20" s="33"/>
       <c r="N20" s="9"/>
-      <c r="O20" s="9" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P20" s="9" t="e">
-        <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q20" s="9" t="e">
-        <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="O20" s="9"/>
+      <c r="P20" s="9"/>
+      <c r="Q20" s="9"/>
       <c r="R20" s="57"/>
       <c r="S20" s="43"/>
       <c r="T20" s="43"/>
@@ -1992,42 +1656,18 @@
       <c r="C21" s="7"/>
       <c r="D21" s="33"/>
       <c r="E21" s="33"/>
-      <c r="F21" s="108">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
+      <c r="F21" s="108"/>
       <c r="G21" s="127"/>
-      <c r="H21" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I21" s="94" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="H21" s="9"/>
+      <c r="I21" s="94"/>
       <c r="J21" s="33"/>
-      <c r="K21" s="100" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L21" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="K21" s="100"/>
+      <c r="L21" s="9"/>
       <c r="M21" s="33"/>
       <c r="N21" s="9"/>
-      <c r="O21" s="9" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P21" s="9" t="e">
-        <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q21" s="9" t="e">
-        <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="O21" s="9"/>
+      <c r="P21" s="9"/>
+      <c r="Q21" s="9"/>
       <c r="R21" s="57"/>
       <c r="S21" s="43"/>
       <c r="T21" s="43"/>
@@ -2040,42 +1680,18 @@
       <c r="C22" s="7"/>
       <c r="D22" s="33"/>
       <c r="E22" s="33"/>
-      <c r="F22" s="108">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
+      <c r="F22" s="108"/>
       <c r="G22" s="127"/>
-      <c r="H22" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I22" s="94" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="H22" s="9"/>
+      <c r="I22" s="94"/>
       <c r="J22" s="33"/>
-      <c r="K22" s="100" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L22" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="K22" s="100"/>
+      <c r="L22" s="9"/>
       <c r="M22" s="33"/>
       <c r="N22" s="9"/>
-      <c r="O22" s="9" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P22" s="9" t="e">
-        <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q22" s="9" t="e">
-        <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="O22" s="9"/>
+      <c r="P22" s="9"/>
+      <c r="Q22" s="9"/>
       <c r="R22" s="57"/>
       <c r="S22" s="43"/>
       <c r="T22" s="43"/>
@@ -2088,42 +1704,18 @@
       <c r="C23" s="7"/>
       <c r="D23" s="33"/>
       <c r="E23" s="33"/>
-      <c r="F23" s="108">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
+      <c r="F23" s="108"/>
       <c r="G23" s="127"/>
-      <c r="H23" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I23" s="94" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="H23" s="9"/>
+      <c r="I23" s="94"/>
       <c r="J23" s="33"/>
-      <c r="K23" s="100" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L23" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="K23" s="100"/>
+      <c r="L23" s="9"/>
       <c r="M23" s="33"/>
       <c r="N23" s="9"/>
-      <c r="O23" s="9" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P23" s="9" t="e">
-        <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q23" s="9" t="e">
-        <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="O23" s="9"/>
+      <c r="P23" s="9"/>
+      <c r="Q23" s="9"/>
       <c r="R23" s="57"/>
       <c r="S23" s="43"/>
       <c r="T23" s="43"/>
@@ -2136,42 +1728,18 @@
       <c r="C24" s="7"/>
       <c r="D24" s="33"/>
       <c r="E24" s="33"/>
-      <c r="F24" s="108">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
+      <c r="F24" s="108"/>
       <c r="G24" s="127"/>
-      <c r="H24" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I24" s="94" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="H24" s="9"/>
+      <c r="I24" s="94"/>
       <c r="J24" s="33"/>
-      <c r="K24" s="100" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L24" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="K24" s="100"/>
+      <c r="L24" s="9"/>
       <c r="M24" s="33"/>
       <c r="N24" s="9"/>
-      <c r="O24" s="9" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P24" s="9" t="e">
-        <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q24" s="9" t="e">
-        <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="O24" s="9"/>
+      <c r="P24" s="9"/>
+      <c r="Q24" s="9"/>
       <c r="R24" s="57"/>
       <c r="S24" s="43"/>
       <c r="T24" s="43"/>
@@ -2184,42 +1752,18 @@
       <c r="C25" s="7"/>
       <c r="D25" s="33"/>
       <c r="E25" s="33"/>
-      <c r="F25" s="108">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
+      <c r="F25" s="108"/>
       <c r="G25" s="127"/>
-      <c r="H25" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I25" s="94" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="H25" s="9"/>
+      <c r="I25" s="94"/>
       <c r="J25" s="33"/>
-      <c r="K25" s="100" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L25" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="K25" s="100"/>
+      <c r="L25" s="9"/>
       <c r="M25" s="33"/>
       <c r="N25" s="9"/>
-      <c r="O25" s="9" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P25" s="9" t="e">
-        <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q25" s="9" t="e">
-        <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="O25" s="9"/>
+      <c r="P25" s="9"/>
+      <c r="Q25" s="9"/>
       <c r="R25" s="57"/>
       <c r="S25" s="43"/>
       <c r="T25" s="43"/>
@@ -2232,42 +1776,18 @@
       <c r="C26" s="7"/>
       <c r="D26" s="33"/>
       <c r="E26" s="33"/>
-      <c r="F26" s="108">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
+      <c r="F26" s="108"/>
       <c r="G26" s="127"/>
-      <c r="H26" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I26" s="94" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="H26" s="9"/>
+      <c r="I26" s="94"/>
       <c r="J26" s="33"/>
-      <c r="K26" s="100" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L26" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="K26" s="100"/>
+      <c r="L26" s="9"/>
       <c r="M26" s="33"/>
       <c r="N26" s="9"/>
-      <c r="O26" s="9" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P26" s="9" t="e">
-        <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q26" s="9" t="e">
-        <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="O26" s="9"/>
+      <c r="P26" s="9"/>
+      <c r="Q26" s="9"/>
       <c r="R26" s="57"/>
       <c r="S26" s="43"/>
       <c r="T26" s="43"/>
@@ -2280,42 +1800,18 @@
       <c r="C27" s="7"/>
       <c r="D27" s="33"/>
       <c r="E27" s="33"/>
-      <c r="F27" s="108">
-        <f>D27+E27</f>
-        <v>0</v>
-      </c>
+      <c r="F27" s="108"/>
       <c r="G27" s="127"/>
-      <c r="H27" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I27" s="94" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="H27" s="9"/>
+      <c r="I27" s="94"/>
       <c r="J27" s="33"/>
-      <c r="K27" s="100" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L27" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="K27" s="100"/>
+      <c r="L27" s="9"/>
       <c r="M27" s="33"/>
       <c r="N27" s="9"/>
-      <c r="O27" s="9" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P27" s="9" t="e">
-        <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q27" s="9" t="e">
-        <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="O27" s="9"/>
+      <c r="P27" s="9"/>
+      <c r="Q27" s="9"/>
       <c r="R27" s="57"/>
       <c r="S27" s="33"/>
       <c r="T27" s="33"/>
@@ -2328,42 +1824,18 @@
       <c r="C28" s="7"/>
       <c r="D28" s="33"/>
       <c r="E28" s="33"/>
-      <c r="F28" s="108">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
+      <c r="F28" s="108"/>
       <c r="G28" s="127"/>
-      <c r="H28" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I28" s="94" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="H28" s="9"/>
+      <c r="I28" s="94"/>
       <c r="J28" s="33"/>
-      <c r="K28" s="100" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L28" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="K28" s="100"/>
+      <c r="L28" s="9"/>
       <c r="M28" s="33"/>
       <c r="N28" s="9"/>
-      <c r="O28" s="9" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P28" s="9" t="e">
-        <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q28" s="9" t="e">
-        <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="O28" s="9"/>
+      <c r="P28" s="9"/>
+      <c r="Q28" s="9"/>
       <c r="R28" s="57"/>
       <c r="S28" s="33"/>
       <c r="T28" s="33"/>
@@ -2376,42 +1848,18 @@
       <c r="C29" s="7"/>
       <c r="D29" s="33"/>
       <c r="E29" s="33"/>
-      <c r="F29" s="108">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
+      <c r="F29" s="108"/>
       <c r="G29" s="127"/>
-      <c r="H29" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I29" s="94" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="H29" s="9"/>
+      <c r="I29" s="94"/>
       <c r="J29" s="33"/>
-      <c r="K29" s="100" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L29" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="K29" s="100"/>
+      <c r="L29" s="9"/>
       <c r="M29" s="33"/>
       <c r="N29" s="9"/>
-      <c r="O29" s="9" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P29" s="9" t="e">
-        <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q29" s="9" t="e">
-        <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="O29" s="9"/>
+      <c r="P29" s="9"/>
+      <c r="Q29" s="9"/>
       <c r="R29" s="57"/>
       <c r="S29" s="33"/>
       <c r="T29" s="33"/>
@@ -2424,42 +1872,18 @@
       <c r="C30" s="7"/>
       <c r="D30" s="33"/>
       <c r="E30" s="33"/>
-      <c r="F30" s="108">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
+      <c r="F30" s="108"/>
       <c r="G30" s="127"/>
-      <c r="H30" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I30" s="94" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="H30" s="9"/>
+      <c r="I30" s="94"/>
       <c r="J30" s="33"/>
-      <c r="K30" s="100" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L30" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="K30" s="100"/>
+      <c r="L30" s="9"/>
       <c r="M30" s="33"/>
       <c r="N30" s="9"/>
-      <c r="O30" s="9" t="e">
-        <f t="shared" ref="O30:O52" si="11">IF(L30&gt;M30,L30-M30,IF((L30-M30)&lt;-1,"-",0))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P30" s="9" t="e">
-        <f t="shared" ref="P30:P52" si="12">IF(L30&gt;M30,"-",L30-M30)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q30" s="9" t="e">
-        <f t="shared" ref="Q30:Q52" si="13">+F30-L30</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="O30" s="9"/>
+      <c r="P30" s="9"/>
+      <c r="Q30" s="9"/>
       <c r="R30" s="57"/>
       <c r="S30" s="33"/>
       <c r="T30" s="33"/>
@@ -2472,42 +1896,18 @@
       <c r="C31" s="7"/>
       <c r="D31" s="33"/>
       <c r="E31" s="33"/>
-      <c r="F31" s="108">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
+      <c r="F31" s="108"/>
       <c r="G31" s="127"/>
-      <c r="H31" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I31" s="94" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="H31" s="9"/>
+      <c r="I31" s="94"/>
       <c r="J31" s="33"/>
-      <c r="K31" s="100" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L31" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="K31" s="100"/>
+      <c r="L31" s="9"/>
       <c r="M31" s="33"/>
       <c r="N31" s="9"/>
-      <c r="O31" s="9" t="e">
-        <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P31" s="9" t="e">
-        <f t="shared" si="12"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q31" s="9" t="e">
-        <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="O31" s="9"/>
+      <c r="P31" s="9"/>
+      <c r="Q31" s="9"/>
       <c r="R31" s="57"/>
       <c r="S31" s="33"/>
       <c r="T31" s="33"/>
@@ -2520,42 +1920,18 @@
       <c r="C32" s="7"/>
       <c r="D32" s="33"/>
       <c r="E32" s="33"/>
-      <c r="F32" s="108">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
+      <c r="F32" s="108"/>
       <c r="G32" s="127"/>
-      <c r="H32" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I32" s="94" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="H32" s="9"/>
+      <c r="I32" s="94"/>
       <c r="J32" s="33"/>
-      <c r="K32" s="100" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L32" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="K32" s="100"/>
+      <c r="L32" s="9"/>
       <c r="M32" s="33"/>
       <c r="N32" s="9"/>
-      <c r="O32" s="9" t="e">
-        <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P32" s="9" t="e">
-        <f t="shared" si="12"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q32" s="9" t="e">
-        <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="O32" s="9"/>
+      <c r="P32" s="9"/>
+      <c r="Q32" s="9"/>
       <c r="R32" s="57"/>
       <c r="S32" s="33"/>
       <c r="T32" s="33"/>
@@ -2568,42 +1944,18 @@
       <c r="C33" s="7"/>
       <c r="D33" s="33"/>
       <c r="E33" s="33"/>
-      <c r="F33" s="108">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
+      <c r="F33" s="108"/>
       <c r="G33" s="127"/>
-      <c r="H33" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I33" s="94" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="H33" s="9"/>
+      <c r="I33" s="94"/>
       <c r="J33" s="33"/>
-      <c r="K33" s="100" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L33" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="K33" s="100"/>
+      <c r="L33" s="9"/>
       <c r="M33" s="33"/>
       <c r="N33" s="9"/>
-      <c r="O33" s="9" t="e">
-        <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P33" s="9" t="e">
-        <f t="shared" si="12"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q33" s="9" t="e">
-        <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="O33" s="9"/>
+      <c r="P33" s="9"/>
+      <c r="Q33" s="9"/>
       <c r="R33" s="57"/>
       <c r="S33" s="33"/>
       <c r="T33" s="33"/>
@@ -2616,42 +1968,18 @@
       <c r="C34" s="7"/>
       <c r="D34" s="33"/>
       <c r="E34" s="33"/>
-      <c r="F34" s="108">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
+      <c r="F34" s="108"/>
       <c r="G34" s="127"/>
-      <c r="H34" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I34" s="94" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="H34" s="9"/>
+      <c r="I34" s="94"/>
       <c r="J34" s="33"/>
-      <c r="K34" s="100" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L34" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="K34" s="100"/>
+      <c r="L34" s="9"/>
       <c r="M34" s="33"/>
       <c r="N34" s="9"/>
-      <c r="O34" s="9" t="e">
-        <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P34" s="9" t="e">
-        <f t="shared" si="12"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q34" s="9" t="e">
-        <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="O34" s="9"/>
+      <c r="P34" s="9"/>
+      <c r="Q34" s="9"/>
       <c r="R34" s="57"/>
       <c r="S34" s="33"/>
       <c r="T34" s="33"/>
@@ -2664,42 +1992,18 @@
       <c r="C35" s="7"/>
       <c r="D35" s="33"/>
       <c r="E35" s="33"/>
-      <c r="F35" s="108">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
+      <c r="F35" s="108"/>
       <c r="G35" s="127"/>
-      <c r="H35" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I35" s="94" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="H35" s="9"/>
+      <c r="I35" s="94"/>
       <c r="J35" s="33"/>
-      <c r="K35" s="100" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L35" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="K35" s="100"/>
+      <c r="L35" s="9"/>
       <c r="M35" s="33"/>
       <c r="N35" s="9"/>
-      <c r="O35" s="9" t="e">
-        <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P35" s="9" t="e">
-        <f t="shared" si="12"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q35" s="9" t="e">
-        <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="O35" s="9"/>
+      <c r="P35" s="9"/>
+      <c r="Q35" s="9"/>
       <c r="R35" s="57"/>
       <c r="S35" s="33"/>
       <c r="T35" s="33"/>
@@ -2712,42 +2016,18 @@
       <c r="C36" s="7"/>
       <c r="D36" s="33"/>
       <c r="E36" s="33"/>
-      <c r="F36" s="108">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
+      <c r="F36" s="108"/>
       <c r="G36" s="127"/>
-      <c r="H36" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I36" s="94" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="H36" s="9"/>
+      <c r="I36" s="94"/>
       <c r="J36" s="33"/>
-      <c r="K36" s="100" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L36" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="K36" s="100"/>
+      <c r="L36" s="9"/>
       <c r="M36" s="33"/>
       <c r="N36" s="9"/>
-      <c r="O36" s="9" t="e">
-        <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P36" s="9" t="e">
-        <f t="shared" si="12"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q36" s="9" t="e">
-        <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="O36" s="9"/>
+      <c r="P36" s="9"/>
+      <c r="Q36" s="9"/>
       <c r="R36" s="57"/>
       <c r="S36" s="33"/>
       <c r="T36" s="33"/>
@@ -2760,42 +2040,18 @@
       <c r="C37" s="7"/>
       <c r="D37" s="33"/>
       <c r="E37" s="33"/>
-      <c r="F37" s="108">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
+      <c r="F37" s="108"/>
       <c r="G37" s="127"/>
-      <c r="H37" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I37" s="94" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="H37" s="9"/>
+      <c r="I37" s="94"/>
       <c r="J37" s="33"/>
-      <c r="K37" s="100" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L37" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="K37" s="100"/>
+      <c r="L37" s="9"/>
       <c r="M37" s="33"/>
       <c r="N37" s="9"/>
-      <c r="O37" s="9" t="e">
-        <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P37" s="9" t="e">
-        <f t="shared" si="12"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q37" s="9" t="e">
-        <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="O37" s="9"/>
+      <c r="P37" s="9"/>
+      <c r="Q37" s="9"/>
       <c r="R37" s="57"/>
       <c r="S37" s="33"/>
       <c r="T37" s="33"/>
@@ -2808,42 +2064,18 @@
       <c r="C38" s="7"/>
       <c r="D38" s="33"/>
       <c r="E38" s="33"/>
-      <c r="F38" s="108">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
+      <c r="F38" s="108"/>
       <c r="G38" s="127"/>
-      <c r="H38" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I38" s="94" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="H38" s="9"/>
+      <c r="I38" s="94"/>
       <c r="J38" s="33"/>
-      <c r="K38" s="100" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L38" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="K38" s="100"/>
+      <c r="L38" s="9"/>
       <c r="M38" s="33"/>
       <c r="N38" s="9"/>
-      <c r="O38" s="9" t="e">
-        <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P38" s="9" t="e">
-        <f t="shared" si="12"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q38" s="9" t="e">
-        <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="O38" s="9"/>
+      <c r="P38" s="9"/>
+      <c r="Q38" s="9"/>
       <c r="R38" s="57"/>
       <c r="S38" s="33"/>
       <c r="T38" s="33"/>
@@ -2856,42 +2088,18 @@
       <c r="C39" s="7"/>
       <c r="D39" s="33"/>
       <c r="E39" s="33"/>
-      <c r="F39" s="108">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
+      <c r="F39" s="108"/>
       <c r="G39" s="127"/>
-      <c r="H39" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I39" s="94" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="H39" s="9"/>
+      <c r="I39" s="94"/>
       <c r="J39" s="33"/>
-      <c r="K39" s="100" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L39" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="K39" s="100"/>
+      <c r="L39" s="9"/>
       <c r="M39" s="33"/>
       <c r="N39" s="9"/>
-      <c r="O39" s="9" t="e">
-        <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P39" s="9" t="e">
-        <f t="shared" si="12"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q39" s="9" t="e">
-        <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="O39" s="9"/>
+      <c r="P39" s="9"/>
+      <c r="Q39" s="9"/>
       <c r="R39" s="57"/>
       <c r="S39" s="33"/>
       <c r="T39" s="33"/>
@@ -2904,42 +2112,18 @@
       <c r="C40" s="7"/>
       <c r="D40" s="33"/>
       <c r="E40" s="33"/>
-      <c r="F40" s="108">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
+      <c r="F40" s="108"/>
       <c r="G40" s="127"/>
-      <c r="H40" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I40" s="94" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="H40" s="9"/>
+      <c r="I40" s="94"/>
       <c r="J40" s="33"/>
-      <c r="K40" s="100" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L40" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="K40" s="100"/>
+      <c r="L40" s="9"/>
       <c r="M40" s="33"/>
       <c r="N40" s="9"/>
-      <c r="O40" s="9" t="e">
-        <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P40" s="9" t="e">
-        <f t="shared" si="12"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q40" s="9" t="e">
-        <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="O40" s="9"/>
+      <c r="P40" s="9"/>
+      <c r="Q40" s="9"/>
       <c r="R40" s="57"/>
       <c r="S40" s="33"/>
       <c r="T40" s="33"/>
@@ -2952,42 +2136,18 @@
       <c r="C41" s="7"/>
       <c r="D41" s="33"/>
       <c r="E41" s="33"/>
-      <c r="F41" s="108">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
+      <c r="F41" s="108"/>
       <c r="G41" s="127"/>
-      <c r="H41" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I41" s="94" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="H41" s="9"/>
+      <c r="I41" s="94"/>
       <c r="J41" s="33"/>
-      <c r="K41" s="100" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L41" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="K41" s="100"/>
+      <c r="L41" s="9"/>
       <c r="M41" s="33"/>
       <c r="N41" s="9"/>
-      <c r="O41" s="9" t="e">
-        <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P41" s="9" t="e">
-        <f t="shared" si="12"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q41" s="9" t="e">
-        <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="O41" s="9"/>
+      <c r="P41" s="9"/>
+      <c r="Q41" s="9"/>
       <c r="R41" s="57"/>
       <c r="S41" s="33"/>
       <c r="T41" s="33"/>
@@ -3000,42 +2160,18 @@
       <c r="C42" s="7"/>
       <c r="D42" s="33"/>
       <c r="E42" s="33"/>
-      <c r="F42" s="108">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
+      <c r="F42" s="108"/>
       <c r="G42" s="127"/>
-      <c r="H42" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I42" s="94" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="H42" s="9"/>
+      <c r="I42" s="94"/>
       <c r="J42" s="33"/>
-      <c r="K42" s="100" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L42" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="K42" s="100"/>
+      <c r="L42" s="9"/>
       <c r="M42" s="33"/>
       <c r="N42" s="9"/>
-      <c r="O42" s="9" t="e">
-        <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P42" s="9" t="e">
-        <f t="shared" si="12"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q42" s="9" t="e">
-        <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="O42" s="9"/>
+      <c r="P42" s="9"/>
+      <c r="Q42" s="9"/>
       <c r="R42" s="57"/>
       <c r="S42" s="33"/>
       <c r="T42" s="33"/>
@@ -3048,42 +2184,18 @@
       <c r="C43" s="7"/>
       <c r="D43" s="33"/>
       <c r="E43" s="33"/>
-      <c r="F43" s="108">
-        <f>D43+E43</f>
-        <v>0</v>
-      </c>
+      <c r="F43" s="108"/>
       <c r="G43" s="127"/>
-      <c r="H43" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I43" s="94" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="H43" s="9"/>
+      <c r="I43" s="94"/>
       <c r="J43" s="33"/>
-      <c r="K43" s="100" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L43" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="K43" s="100"/>
+      <c r="L43" s="9"/>
       <c r="M43" s="33"/>
       <c r="N43" s="9"/>
-      <c r="O43" s="9" t="e">
-        <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P43" s="9" t="e">
-        <f t="shared" si="12"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q43" s="9" t="e">
-        <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="O43" s="9"/>
+      <c r="P43" s="9"/>
+      <c r="Q43" s="9"/>
       <c r="R43" s="57"/>
       <c r="S43" s="33"/>
       <c r="T43" s="33"/>
@@ -3096,42 +2208,18 @@
       <c r="C44" s="7"/>
       <c r="D44" s="33"/>
       <c r="E44" s="33"/>
-      <c r="F44" s="108">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
+      <c r="F44" s="108"/>
       <c r="G44" s="127"/>
-      <c r="H44" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I44" s="94" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="H44" s="9"/>
+      <c r="I44" s="94"/>
       <c r="J44" s="33"/>
-      <c r="K44" s="100" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L44" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="K44" s="100"/>
+      <c r="L44" s="9"/>
       <c r="M44" s="33"/>
       <c r="N44" s="9"/>
-      <c r="O44" s="9" t="e">
-        <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P44" s="9" t="e">
-        <f t="shared" si="12"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q44" s="9" t="e">
-        <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="O44" s="9"/>
+      <c r="P44" s="9"/>
+      <c r="Q44" s="9"/>
       <c r="R44" s="57"/>
       <c r="S44" s="33"/>
       <c r="T44" s="33"/>
@@ -3144,42 +2232,18 @@
       <c r="C45" s="7"/>
       <c r="D45" s="33"/>
       <c r="E45" s="33"/>
-      <c r="F45" s="108">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
+      <c r="F45" s="108"/>
       <c r="G45" s="127"/>
-      <c r="H45" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I45" s="94" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="H45" s="9"/>
+      <c r="I45" s="94"/>
       <c r="J45" s="33"/>
-      <c r="K45" s="100" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L45" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="K45" s="100"/>
+      <c r="L45" s="9"/>
       <c r="M45" s="33"/>
       <c r="N45" s="9"/>
-      <c r="O45" s="9" t="e">
-        <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P45" s="9" t="e">
-        <f t="shared" si="12"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q45" s="9" t="e">
-        <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="O45" s="9"/>
+      <c r="P45" s="9"/>
+      <c r="Q45" s="9"/>
       <c r="R45" s="57"/>
       <c r="S45" s="33"/>
       <c r="T45" s="33"/>
@@ -3192,42 +2256,18 @@
       <c r="C46" s="7"/>
       <c r="D46" s="33"/>
       <c r="E46" s="33"/>
-      <c r="F46" s="108">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
+      <c r="F46" s="108"/>
       <c r="G46" s="127"/>
-      <c r="H46" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I46" s="94" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="H46" s="9"/>
+      <c r="I46" s="94"/>
       <c r="J46" s="33"/>
-      <c r="K46" s="100" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L46" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="K46" s="100"/>
+      <c r="L46" s="9"/>
       <c r="M46" s="33"/>
       <c r="N46" s="9"/>
-      <c r="O46" s="9" t="e">
-        <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P46" s="9" t="e">
-        <f t="shared" si="12"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q46" s="9" t="e">
-        <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="O46" s="9"/>
+      <c r="P46" s="9"/>
+      <c r="Q46" s="9"/>
       <c r="R46" s="57"/>
       <c r="S46" s="33"/>
       <c r="T46" s="33"/>
@@ -3240,42 +2280,18 @@
       <c r="C47" s="7"/>
       <c r="D47" s="33"/>
       <c r="E47" s="33"/>
-      <c r="F47" s="108">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
+      <c r="F47" s="108"/>
       <c r="G47" s="127"/>
-      <c r="H47" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I47" s="94" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="H47" s="9"/>
+      <c r="I47" s="94"/>
       <c r="J47" s="33"/>
-      <c r="K47" s="100" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L47" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="K47" s="100"/>
+      <c r="L47" s="9"/>
       <c r="M47" s="33"/>
       <c r="N47" s="9"/>
-      <c r="O47" s="9" t="e">
-        <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P47" s="9" t="e">
-        <f t="shared" si="12"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q47" s="9" t="e">
-        <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="O47" s="9"/>
+      <c r="P47" s="9"/>
+      <c r="Q47" s="9"/>
       <c r="R47" s="57"/>
       <c r="S47" s="33"/>
       <c r="T47" s="33"/>
@@ -3288,42 +2304,18 @@
       <c r="C48" s="7"/>
       <c r="D48" s="33"/>
       <c r="E48" s="33"/>
-      <c r="F48" s="108">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
+      <c r="F48" s="108"/>
       <c r="G48" s="127"/>
-      <c r="H48" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I48" s="94" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="H48" s="9"/>
+      <c r="I48" s="94"/>
       <c r="J48" s="33"/>
-      <c r="K48" s="100" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L48" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="K48" s="100"/>
+      <c r="L48" s="9"/>
       <c r="M48" s="33"/>
       <c r="N48" s="9"/>
-      <c r="O48" s="9" t="e">
-        <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P48" s="9" t="e">
-        <f t="shared" si="12"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q48" s="9" t="e">
-        <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="O48" s="9"/>
+      <c r="P48" s="9"/>
+      <c r="Q48" s="9"/>
       <c r="R48" s="57"/>
       <c r="S48" s="33"/>
       <c r="T48" s="33"/>
@@ -3336,42 +2328,18 @@
       <c r="C49" s="7"/>
       <c r="D49" s="33"/>
       <c r="E49" s="33"/>
-      <c r="F49" s="108">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
+      <c r="F49" s="108"/>
       <c r="G49" s="127"/>
-      <c r="H49" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I49" s="94" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="H49" s="9"/>
+      <c r="I49" s="94"/>
       <c r="J49" s="33"/>
-      <c r="K49" s="100" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L49" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="K49" s="100"/>
+      <c r="L49" s="9"/>
       <c r="M49" s="33"/>
       <c r="N49" s="9"/>
-      <c r="O49" s="9" t="e">
-        <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P49" s="9" t="e">
-        <f t="shared" si="12"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q49" s="9" t="e">
-        <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="O49" s="9"/>
+      <c r="P49" s="9"/>
+      <c r="Q49" s="9"/>
       <c r="R49" s="57"/>
       <c r="S49" s="33"/>
       <c r="T49" s="33"/>
@@ -3384,42 +2352,18 @@
       <c r="C50" s="7"/>
       <c r="D50" s="33"/>
       <c r="E50" s="33"/>
-      <c r="F50" s="108">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
+      <c r="F50" s="108"/>
       <c r="G50" s="127"/>
-      <c r="H50" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I50" s="94" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="H50" s="9"/>
+      <c r="I50" s="94"/>
       <c r="J50" s="33"/>
-      <c r="K50" s="100" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L50" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="K50" s="100"/>
+      <c r="L50" s="9"/>
       <c r="M50" s="33"/>
       <c r="N50" s="9"/>
-      <c r="O50" s="9" t="e">
-        <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P50" s="9" t="e">
-        <f t="shared" si="12"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q50" s="9" t="e">
-        <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="O50" s="9"/>
+      <c r="P50" s="9"/>
+      <c r="Q50" s="9"/>
       <c r="R50" s="57"/>
       <c r="S50" s="33"/>
       <c r="T50" s="33"/>
@@ -3432,42 +2376,18 @@
       <c r="C51" s="7"/>
       <c r="D51" s="33"/>
       <c r="E51" s="33"/>
-      <c r="F51" s="108">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
+      <c r="F51" s="108"/>
       <c r="G51" s="127"/>
-      <c r="H51" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I51" s="94" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="H51" s="9"/>
+      <c r="I51" s="94"/>
       <c r="J51" s="33"/>
-      <c r="K51" s="100" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L51" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="K51" s="100"/>
+      <c r="L51" s="9"/>
       <c r="M51" s="33"/>
       <c r="N51" s="9"/>
-      <c r="O51" s="9" t="e">
-        <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P51" s="9" t="e">
-        <f t="shared" si="12"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q51" s="9" t="e">
-        <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="O51" s="9"/>
+      <c r="P51" s="9"/>
+      <c r="Q51" s="9"/>
       <c r="R51" s="57"/>
       <c r="S51" s="33"/>
       <c r="T51" s="33"/>
@@ -3480,42 +2400,18 @@
       <c r="C52" s="7"/>
       <c r="D52" s="33"/>
       <c r="E52" s="33"/>
-      <c r="F52" s="108">
-        <f>D52+E52</f>
-        <v>0</v>
-      </c>
+      <c r="F52" s="108"/>
       <c r="G52" s="127"/>
-      <c r="H52" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I52" s="94" t="e">
-        <f>H52/G52</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="H52" s="9"/>
+      <c r="I52" s="94"/>
       <c r="J52" s="33"/>
-      <c r="K52" s="100" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L52" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="K52" s="100"/>
+      <c r="L52" s="9"/>
       <c r="M52" s="33"/>
       <c r="N52" s="9"/>
-      <c r="O52" s="9" t="e">
-        <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P52" s="9" t="e">
-        <f t="shared" si="12"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q52" s="9" t="e">
-        <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="O52" s="9"/>
+      <c r="P52" s="9"/>
+      <c r="Q52" s="9"/>
       <c r="R52" s="57"/>
       <c r="S52" s="33"/>
       <c r="T52" s="33"/>
@@ -3528,16 +2424,10 @@
       <c r="C53" s="7"/>
       <c r="D53" s="33"/>
       <c r="E53" s="33"/>
-      <c r="F53" s="107">
-        <f>D53+E53</f>
-        <v>0</v>
-      </c>
+      <c r="F53" s="107"/>
       <c r="G53" s="127"/>
       <c r="H53" s="9"/>
-      <c r="I53" s="132" t="e">
-        <f>H53/G53</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="I53" s="132"/>
       <c r="J53" s="33"/>
       <c r="K53" s="100"/>
       <c r="L53" s="9"/>

</xml_diff>